<commit_message>
grouped data with country, and uni name
</commit_message>
<xml_diff>
--- a/server/exchange.xlsx
+++ b/server/exchange.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwonseoyoung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCB25E1-9029-C94D-BAFA-BB86AD0C9278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A67583-80FB-9842-BCA7-19AA74DE3031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="1625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3078" uniqueCount="1642">
   <si>
     <t>TAIWAN</t>
   </si>
@@ -5274,35 +5274,86 @@
     <t>https://drive.google.com/open?id=1q6q9VEzw7huyvzg10JLClErCoV9ud4c8</t>
   </si>
   <si>
+    <t>03. Does your institution have multiple campuses?</t>
+  </si>
+  <si>
+    <t>- Please write all campuses SKKU students can go to.
+- Please specify majors by the campus.</t>
+  </si>
+  <si>
+    <t>지원 가능 전공/단과대
+* 우리 대학
+원전공, 복수전공 기준</t>
+  </si>
+  <si>
+    <t>해외대학 수학 전공
+* 파견 시 해외대학에서 선택 가능한 전공</t>
+  </si>
+  <si>
+    <t>2024-2 TO</t>
+  </si>
+  <si>
+    <t>Email address for SKKU students' inquiries</t>
+  </si>
+  <si>
+    <t>09. The website link for the exchange program (If any)</t>
+  </si>
+  <si>
+    <t>10. Please specify language requirements if there are any.</t>
+  </si>
+  <si>
+    <t>11. Do you accept graduate-level students?</t>
+  </si>
+  <si>
+    <t>12. Do you accept one-year exchange students starting from fall semester of 2024?</t>
+  </si>
+  <si>
+    <t>13. Do you allow students to take courses outside their major?</t>
+  </si>
+  <si>
+    <t>14. Minimum GPA to join the exchange program at your institution
+- Please specify the grading scale as well.</t>
+  </si>
+  <si>
+    <t>15. How many semesters do SKKU students have to complete before the spring semester of 2024?</t>
+  </si>
+  <si>
+    <t>16. MINIMUM credits/ECTS that SKKU students have to take at your institution</t>
+  </si>
+  <si>
+    <t>17. MAXIMUM credits/ECTS that SKKU students can take at your institution</t>
+  </si>
+  <si>
+    <t>18. Nomination deadline for 2024 Spring semester</t>
+  </si>
+  <si>
+    <t>19. Application deadline for 2024 Spring semester</t>
+  </si>
+  <si>
+    <t>21. Please specify if there are any restrictions on choosing majors.</t>
+  </si>
+  <si>
+    <t>22. Plesae specify if there are any restrictions on choosing courses.</t>
+  </si>
+  <si>
+    <t>23. How do you share course catalog to SKKU students?</t>
+  </si>
+  <si>
+    <t>24. Additional information for SKKU students to be aware of (if available)</t>
+  </si>
+  <si>
+    <t>Factsheet for 2024 Fall</t>
+  </si>
+  <si>
     <t>Country</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>University name</t>
+    <t>University Name</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Campus</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Major</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Department</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grade</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact </t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Website</t>
+    <t>Location/Campus</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -5314,7 +5365,7 @@
     <numFmt numFmtId="176" formatCode="yyyy\.\ m\.\ d"/>
     <numFmt numFmtId="177" formatCode="m\-d"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -5412,6 +5463,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5439,7 +5513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5483,6 +5557,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -5701,13 +5781,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X820"/>
+  <dimension ref="A1:Z820"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5722,33 +5802,85 @@
     <col min="10" max="10" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>1617</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="E1" s="26" t="s">
         <v>1618</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="F1" s="26" t="s">
         <v>1619</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>1620</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>1621</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>1622</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>1623</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="K1" s="25" t="s">
         <v>1624</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="19.5" customHeight="1">
+      <c r="L1" s="25" t="s">
+        <v>1625</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>1626</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>1627</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>1628</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>1629</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>1630</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>1631</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>1632</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>1633</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>1634</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>1635</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>1636</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>1637</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>1638</v>
+      </c>
+      <c r="Z1" s="24"/>
+    </row>
+    <row r="2" spans="1:26" ht="19.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5818,7 +5950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1">
+    <row r="3" spans="1:26" ht="19.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -5884,7 +6016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1">
+    <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -5954,7 +6086,7 @@
       </c>
       <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:24" ht="19.5" customHeight="1">
+    <row r="5" spans="1:26" ht="19.5" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
@@ -6026,7 +6158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="19.5" customHeight="1">
+    <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -6096,7 +6228,7 @@
       <c r="W6" s="7"/>
       <c r="X6" s="10"/>
     </row>
-    <row r="7" spans="1:24" ht="19.5" customHeight="1">
+    <row r="7" spans="1:26" ht="19.5" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -6168,7 +6300,7 @@
       </c>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="19.5" customHeight="1">
+    <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
@@ -6240,7 +6372,7 @@
       </c>
       <c r="X8" s="10"/>
     </row>
-    <row r="9" spans="1:24" ht="19.5" customHeight="1">
+    <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -6312,7 +6444,7 @@
       </c>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="19.5" customHeight="1">
+    <row r="10" spans="1:26" ht="19.5" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>94</v>
       </c>
@@ -6386,7 +6518,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1">
+    <row r="11" spans="1:26" ht="19.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -6460,7 +6592,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1">
+    <row r="12" spans="1:26" ht="19.5" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>122</v>
       </c>
@@ -6530,7 +6662,7 @@
       </c>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="19.5" customHeight="1">
+    <row r="13" spans="1:26" ht="19.5" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>132</v>
       </c>
@@ -6602,7 +6734,7 @@
       </c>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="19.5" customHeight="1">
+    <row r="14" spans="1:26" ht="19.5" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>141</v>
       </c>
@@ -6672,7 +6804,7 @@
       <c r="W14" s="7"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="19.5" customHeight="1">
+    <row r="15" spans="1:26" ht="19.5" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>150</v>
       </c>
@@ -6742,7 +6874,7 @@
       </c>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="19.5" customHeight="1">
+    <row r="16" spans="1:26" ht="19.5" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>122</v>
       </c>
@@ -20745,11 +20877,11 @@
   <customSheetViews>
     <customSheetView guid="{67FC2E35-4B0B-45C0-A1F3-FDF8F409A3AC}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:E2" xr:uid="{3D18142A-106A-0E4E-915A-2083F7E964F7}"/>
+      <autoFilter ref="A1:E2" xr:uid="{2ACCCEB4-7B1F-004A-9F3C-DB69754E5B61}"/>
     </customSheetView>
     <customSheetView guid="{90E31945-B7C6-4DC3-92D0-CE1C4D3678D0}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A6:Y173" xr:uid="{598986A9-1CFD-6441-B2FD-5945D9FC6A04}">
+      <autoFilter ref="A6:Y173" xr:uid="{BE33AFD4-DE81-404F-AAEA-C241225A5607}">
         <filterColumn colId="18">
           <filters>
             <filter val="2/20/2024"/>
@@ -20791,7 +20923,7 @@
     </customSheetView>
     <customSheetView guid="{6D4B485E-E721-4BAE-A3C1-3F0B123327D2}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A6:Y173" xr:uid="{E297C928-C944-D54E-A3D8-B4B4EFD8E2BA}"/>
+      <autoFilter ref="A6:Y173" xr:uid="{9C6D20EA-8DA7-5F4F-8AD2-B16207B90811}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="13" type="noConversion"/>

</xml_diff>